<commit_message>
Adding most of the impl and more tests
</commit_message>
<xml_diff>
--- a/src/test/resources/com/kcbierco/DatesFromFormula.xlsx
+++ b/src/test/resources/com/kcbierco/DatesFromFormula.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Test" sheetId="1" r:id="rId1"/>
+    <sheet name="Inputs(1)" sheetId="2" r:id="rId1"/>
+    <sheet name="Inputs(2)" sheetId="3" r:id="rId2"/>
+    <sheet name="Cellar Record" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,16 +21,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Tank 334</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Tank 34</t>
+  </si>
+  <si>
+    <t>Check 1</t>
+  </si>
+  <si>
+    <t>Check 2</t>
+  </si>
+  <si>
+    <t>Check 3</t>
+  </si>
+  <si>
+    <t>Keep</t>
+  </si>
+  <si>
+    <t>Checking</t>
+  </si>
+  <si>
+    <t>Until</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Three </t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -52,6 +81,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -61,12 +98,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -75,9 +127,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -411,39 +465,183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E6"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="3" spans="2:5">
-      <c r="B3" s="1">
+    <row r="4" spans="3:3">
+      <c r="C4" s="1">
         <f ca="1">TODAY()</f>
-        <v>42400</v>
-      </c>
-      <c r="E3" t="s">
+        <v>42406</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:I36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="3" spans="1:9">
+      <c r="B3" s="1"/>
+      <c r="G3" s="1">
+        <f ca="1">'Inputs(2)'!C4</f>
+        <v>42406</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="B5" s="1"/>
+      <c r="I5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="1">
-        <f ca="1">TODAY() + 1</f>
-        <v>42401</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="1">
-        <f ca="1">TODAY() + 2</f>
-        <v>42402</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="1">
-        <f ca="1">TODAY() + 3</f>
-        <v>42403</v>
+    <row r="6" spans="1:9">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="E13" s="1">
+        <f ca="1">G3</f>
+        <v>42406</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
+        <f ca="1">E13+2</f>
+        <v>42408</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1">
+        <f ca="1">E13+4</f>
+        <v>42410</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1">
+        <f ca="1">E13+6</f>
+        <v>42412</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1">
+        <f ca="1">E13+7</f>
+        <v>42413</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1">
+        <f ca="1">E13+8</f>
+        <v>42414</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1">
+        <f ca="1">E13+9</f>
+        <v>42415</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1">
+        <f ca="1">E13+10</f>
+        <v>42416</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1">
+        <f ca="1">E13+11</f>
+        <v>42417</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="D31" s="1">
+        <f ca="1">TODAY()</f>
+        <v>42406</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" ht="18">
+      <c r="D33" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="D34" s="3">
+        <f ca="1">D31+1</f>
+        <v>42407</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="D35" s="3">
+        <f ca="1">D31+2</f>
+        <v>42408</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4">
+      <c r="D36" s="3">
+        <f ca="1">D31+4</f>
+        <v>42410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>